<commit_message>
Attempt to add taxes on gasoline
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Fuel_Price_Import_ELC_TS24.xlsx
+++ b/SuppXLS/Scen_Fuel_Price_Import_ELC_TS24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kroann\Documents\Samarbeten\VTI\City_TRA_STHLM-main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabGren\Work Folders\Documents\TransportElModellSthlm\SimpleModel\City_TRA_STHLM_ts\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F862522B-6CCF-48ED-99B7-2A3C50093D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1900F6C0-7087-4C8D-8B4A-2A43B449267F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabriella Grenander</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{F8BFB6E5-68E4-4487-9FA1-73EDAE8949D4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Grenander:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dummy values</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{8E0E7860-30F2-4442-9FA6-208A0F774471}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Grenander:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dummy values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
@@ -165,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +257,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -310,6 +381,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,23 +649,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H2" s="9" t="s">
         <v>39</v>
       </c>
@@ -598,13 +673,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -627,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -644,7 +719,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -665,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -682,7 +757,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,12 +774,12 @@
         <v>999</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
@@ -730,7 +805,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -751,7 +826,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -772,7 +847,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
@@ -793,7 +868,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -814,7 +889,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -835,7 +910,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -856,7 +931,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
@@ -877,7 +952,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
@@ -898,7 +973,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -919,7 +994,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -940,7 +1015,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
@@ -961,7 +1036,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
@@ -982,7 +1057,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1003,7 +1078,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
@@ -1024,7 +1099,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1045,7 +1120,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1066,7 +1141,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1087,7 +1162,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1108,7 +1183,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1129,7 +1204,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1225,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1171,7 +1246,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1267,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
@@ -1213,7 +1288,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1237,5 +1312,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>